<commit_message>
add TSR and email address
</commit_message>
<xml_diff>
--- a/templates/dataplant/PRIDE.xlsx
+++ b/templates/dataplant/PRIDE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>mailto:maus@nfdi4plants.org</t>
+  </si>
+  <si>
+    <t>s.eggels@fz-juelich.de</t>
   </si>
   <si>
     <t>Author Phone</t>
@@ -702,11 +705,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -742,67 +748,70 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
       </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -818,72 +827,72 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>